<commit_message>
Publish with updated snapshot
</commit_message>
<xml_diff>
--- a/docs/UKCore-Observation.xlsx
+++ b/docs/UKCore-Observation.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$240</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8461" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8908" uniqueCount="733">
   <si>
     <t>Path</t>
   </si>
@@ -2214,6 +2214,39 @@
   <si>
     <t>&lt; 363787002 |Observable entity| OR  &lt; 386053000 |Evaluation procedure|</t>
+  </si>
+  <si>
+    <t>Observation.component.code.id</t>
+  </si>
+  <si>
+    <t>Observation.component.code.extension</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.id</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.extension</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.system</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.version</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.code</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.display</t>
+  </si>
+  <si>
+    <t>Observation.component.code.coding.userSelected</t>
+  </si>
+  <si>
+    <t>Observation.component.code.text</t>
   </si>
   <si>
     <t>Observation.component.value[x]</t>
@@ -2399,7 +2432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO228"/>
+  <dimension ref="A1:AO240"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2408,7 +2441,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="46.2890625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -28723,23 +28756,19 @@
         <v>45</v>
       </c>
       <c r="I225" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J225" t="s" s="2">
-        <v>463</v>
+        <v>57</v>
       </c>
       <c r="K225" t="s" s="2">
-        <v>711</v>
+        <v>122</v>
       </c>
       <c r="L225" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="M225" t="s" s="2">
-        <v>712</v>
-      </c>
-      <c r="N225" t="s" s="2">
-        <v>467</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="M225" s="2"/>
+      <c r="N225" s="2"/>
       <c r="O225" t="s" s="2">
         <v>45</v>
       </c>
@@ -28787,7 +28816,7 @@
         <v>45</v>
       </c>
       <c r="AE225" t="s" s="2">
-        <v>710</v>
+        <v>124</v>
       </c>
       <c r="AF225" t="s" s="2">
         <v>43</v>
@@ -28799,41 +28828,41 @@
         <v>45</v>
       </c>
       <c r="AI225" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ225" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK225" t="s" s="2">
-        <v>713</v>
+        <v>45</v>
       </c>
       <c r="AL225" t="s" s="2">
-        <v>470</v>
+        <v>45</v>
       </c>
       <c r="AM225" t="s" s="2">
-        <v>471</v>
+        <v>125</v>
       </c>
       <c r="AN225" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO225" t="s" s="2">
-        <v>472</v>
+        <v>45</v>
       </c>
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D226" s="2"/>
       <c r="E226" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F226" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G226" t="s" s="2">
         <v>45</v>
@@ -28845,20 +28874,18 @@
         <v>45</v>
       </c>
       <c r="J226" t="s" s="2">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="K226" t="s" s="2">
-        <v>715</v>
+        <v>102</v>
       </c>
       <c r="L226" t="s" s="2">
-        <v>716</v>
+        <v>127</v>
       </c>
       <c r="M226" t="s" s="2">
-        <v>717</v>
-      </c>
-      <c r="N226" t="s" s="2">
-        <v>477</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="N226" s="2"/>
       <c r="O226" t="s" s="2">
         <v>45</v>
       </c>
@@ -28882,43 +28909,43 @@
         <v>45</v>
       </c>
       <c r="W226" t="s" s="2">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="X226" t="s" s="2">
-        <v>478</v>
+        <v>45</v>
       </c>
       <c r="Y226" t="s" s="2">
-        <v>479</v>
+        <v>45</v>
       </c>
       <c r="Z226" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA226" t="s" s="2">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="AB226" t="s" s="2">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="AC226" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD226" t="s" s="2">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="AE226" t="s" s="2">
-        <v>714</v>
+        <v>131</v>
       </c>
       <c r="AF226" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG226" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH226" t="s" s="2">
-        <v>480</v>
+        <v>45</v>
       </c>
       <c r="AI226" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ226" t="s" s="2">
         <v>45</v>
@@ -28927,10 +28954,10 @@
         <v>45</v>
       </c>
       <c r="AL226" t="s" s="2">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="AM226" t="s" s="2">
-        <v>481</v>
+        <v>125</v>
       </c>
       <c r="AN226" t="s" s="2">
         <v>45</v>
@@ -28941,11 +28968,11 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
-        <v>483</v>
+        <v>45</v>
       </c>
       <c r="D227" s="2"/>
       <c r="E227" t="s" s="2">
@@ -28961,22 +28988,22 @@
         <v>45</v>
       </c>
       <c r="I227" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J227" t="s" s="2">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="K227" t="s" s="2">
-        <v>484</v>
+        <v>291</v>
       </c>
       <c r="L227" t="s" s="2">
-        <v>485</v>
+        <v>292</v>
       </c>
       <c r="M227" t="s" s="2">
-        <v>486</v>
+        <v>293</v>
       </c>
       <c r="N227" t="s" s="2">
-        <v>487</v>
+        <v>294</v>
       </c>
       <c r="O227" t="s" s="2">
         <v>45</v>
@@ -29001,31 +29028,29 @@
         <v>45</v>
       </c>
       <c r="W227" t="s" s="2">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="X227" t="s" s="2">
-        <v>488</v>
+        <v>45</v>
       </c>
       <c r="Y227" t="s" s="2">
-        <v>489</v>
+        <v>45</v>
       </c>
       <c r="Z227" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA227" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB227" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="AB227" s="2"/>
       <c r="AC227" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD227" t="s" s="2">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="AE227" t="s" s="2">
-        <v>718</v>
+        <v>296</v>
       </c>
       <c r="AF227" t="s" s="2">
         <v>43</v>
@@ -29043,26 +29068,28 @@
         <v>45</v>
       </c>
       <c r="AK227" t="s" s="2">
-        <v>490</v>
+        <v>45</v>
       </c>
       <c r="AL227" t="s" s="2">
-        <v>491</v>
+        <v>297</v>
       </c>
       <c r="AM227" t="s" s="2">
-        <v>492</v>
+        <v>298</v>
       </c>
       <c r="AN227" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO227" t="s" s="2">
-        <v>493</v>
+        <v>45</v>
       </c>
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>719</v>
-      </c>
-      <c r="B228" s="2"/>
+        <v>712</v>
+      </c>
+      <c r="B228" t="s" s="2">
+        <v>299</v>
+      </c>
       <c r="C228" t="s" s="2">
         <v>45</v>
       </c>
@@ -29080,22 +29107,22 @@
         <v>45</v>
       </c>
       <c r="I228" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J228" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="K228" t="s" s="2">
-        <v>720</v>
+        <v>291</v>
       </c>
       <c r="L228" t="s" s="2">
-        <v>721</v>
+        <v>292</v>
       </c>
       <c r="M228" t="s" s="2">
-        <v>605</v>
+        <v>293</v>
       </c>
       <c r="N228" t="s" s="2">
-        <v>606</v>
+        <v>294</v>
       </c>
       <c r="O228" t="s" s="2">
         <v>45</v>
@@ -29120,13 +29147,13 @@
         <v>45</v>
       </c>
       <c r="W228" t="s" s="2">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="X228" t="s" s="2">
-        <v>45</v>
+        <v>300</v>
       </c>
       <c r="Y228" t="s" s="2">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="Z228" t="s" s="2">
         <v>45</v>
@@ -29144,7 +29171,7 @@
         <v>45</v>
       </c>
       <c r="AE228" t="s" s="2">
-        <v>719</v>
+        <v>296</v>
       </c>
       <c r="AF228" t="s" s="2">
         <v>43</v>
@@ -29165,20 +29192,1436 @@
         <v>45</v>
       </c>
       <c r="AL228" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AM228" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AN228" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO228" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="229" hidden="true">
+      <c r="A229" t="s" s="2">
+        <v>713</v>
+      </c>
+      <c r="B229" s="2"/>
+      <c r="C229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D229" s="2"/>
+      <c r="E229" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F229" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J229" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K229" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L229" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M229" s="2"/>
+      <c r="N229" s="2"/>
+      <c r="O229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P229" s="2"/>
+      <c r="Q229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE229" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AF229" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG229" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM229" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AN229" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO229" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="230" hidden="true">
+      <c r="A230" t="s" s="2">
+        <v>714</v>
+      </c>
+      <c r="B230" s="2"/>
+      <c r="C230" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="D230" s="2"/>
+      <c r="E230" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F230" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J230" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="K230" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="L230" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M230" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="N230" s="2"/>
+      <c r="O230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P230" s="2"/>
+      <c r="Q230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA230" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="AB230" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AC230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD230" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AE230" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF230" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG230" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI230" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AJ230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM230" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AN230" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO230" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="231" hidden="true">
+      <c r="A231" t="s" s="2">
+        <v>715</v>
+      </c>
+      <c r="B231" s="2"/>
+      <c r="C231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D231" s="2"/>
+      <c r="E231" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="F231" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I231" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J231" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="K231" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="L231" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="M231" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="N231" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="O231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P231" s="2"/>
+      <c r="Q231" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="R231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE231" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="AF231" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG231" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI231" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL231" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AM231" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN231" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO231" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="232" hidden="true">
+      <c r="A232" t="s" s="2">
+        <v>716</v>
+      </c>
+      <c r="B232" s="2"/>
+      <c r="C232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D232" s="2"/>
+      <c r="E232" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F232" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I232" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J232" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K232" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L232" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="M232" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="N232" s="2"/>
+      <c r="O232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P232" s="2"/>
+      <c r="Q232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE232" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AF232" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG232" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI232" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL232" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AM232" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="AN232" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO232" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="233" hidden="true">
+      <c r="A233" t="s" s="2">
+        <v>717</v>
+      </c>
+      <c r="B233" s="2"/>
+      <c r="C233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D233" s="2"/>
+      <c r="E233" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="F233" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I233" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J233" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K233" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L233" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M233" s="2"/>
+      <c r="N233" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="O233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P233" s="2"/>
+      <c r="Q233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE233" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AF233" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG233" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI233" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL233" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AM233" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AN233" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO233" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="234" hidden="true">
+      <c r="A234" t="s" s="2">
+        <v>718</v>
+      </c>
+      <c r="B234" s="2"/>
+      <c r="C234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D234" s="2"/>
+      <c r="E234" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="F234" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I234" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J234" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K234" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="L234" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="M234" s="2"/>
+      <c r="N234" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="O234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P234" s="2"/>
+      <c r="Q234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE234" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AF234" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG234" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI234" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL234" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AM234" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="AN234" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO234" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="235" hidden="true">
+      <c r="A235" t="s" s="2">
+        <v>719</v>
+      </c>
+      <c r="B235" s="2"/>
+      <c r="C235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D235" s="2"/>
+      <c r="E235" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F235" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I235" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J235" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="K235" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="L235" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="M235" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="N235" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="O235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P235" s="2"/>
+      <c r="Q235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE235" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AF235" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG235" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI235" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL235" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="AM235" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AN235" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO235" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="236" hidden="true">
+      <c r="A236" t="s" s="2">
+        <v>720</v>
+      </c>
+      <c r="B236" s="2"/>
+      <c r="C236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D236" s="2"/>
+      <c r="E236" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F236" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I236" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J236" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K236" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="L236" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="M236" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="N236" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="O236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P236" s="2"/>
+      <c r="Q236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE236" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AF236" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG236" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI236" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL236" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AM236" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AN236" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO236" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="237" hidden="true">
+      <c r="A237" t="s" s="2">
+        <v>721</v>
+      </c>
+      <c r="B237" s="2"/>
+      <c r="C237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D237" s="2"/>
+      <c r="E237" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F237" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I237" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J237" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="K237" t="s" s="2">
+        <v>722</v>
+      </c>
+      <c r="L237" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="M237" t="s" s="2">
+        <v>723</v>
+      </c>
+      <c r="N237" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="O237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P237" s="2"/>
+      <c r="Q237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE237" t="s" s="2">
+        <v>721</v>
+      </c>
+      <c r="AF237" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG237" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI237" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK237" t="s" s="2">
+        <v>724</v>
+      </c>
+      <c r="AL237" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AM237" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AN237" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO237" t="s" s="2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="238" hidden="true">
+      <c r="A238" t="s" s="2">
+        <v>725</v>
+      </c>
+      <c r="B238" s="2"/>
+      <c r="C238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D238" s="2"/>
+      <c r="E238" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F238" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J238" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="K238" t="s" s="2">
+        <v>726</v>
+      </c>
+      <c r="L238" t="s" s="2">
+        <v>727</v>
+      </c>
+      <c r="M238" t="s" s="2">
+        <v>728</v>
+      </c>
+      <c r="N238" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="O238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P238" s="2"/>
+      <c r="Q238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W238" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="X238" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="Y238" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="Z238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE238" t="s" s="2">
+        <v>725</v>
+      </c>
+      <c r="AF238" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG238" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH238" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="AI238" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL238" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AM238" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="AN238" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO238" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="239" hidden="true">
+      <c r="A239" t="s" s="2">
+        <v>729</v>
+      </c>
+      <c r="B239" s="2"/>
+      <c r="C239" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="D239" s="2"/>
+      <c r="E239" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F239" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J239" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="K239" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="L239" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="M239" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="N239" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="O239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P239" s="2"/>
+      <c r="Q239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W239" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="X239" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="Y239" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="Z239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE239" t="s" s="2">
+        <v>729</v>
+      </c>
+      <c r="AF239" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG239" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI239" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK239" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="AL239" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AM239" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="AN239" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO239" t="s" s="2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="240" hidden="true">
+      <c r="A240" t="s" s="2">
+        <v>730</v>
+      </c>
+      <c r="B240" s="2"/>
+      <c r="C240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D240" s="2"/>
+      <c r="E240" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F240" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K240" t="s" s="2">
+        <v>731</v>
+      </c>
+      <c r="L240" t="s" s="2">
+        <v>732</v>
+      </c>
+      <c r="M240" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="N240" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="O240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P240" s="2"/>
+      <c r="Q240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE240" t="s" s="2">
+        <v>730</v>
+      </c>
+      <c r="AF240" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG240" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI240" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL240" t="s" s="2">
         <v>608</v>
       </c>
-      <c r="AM228" t="s" s="2">
+      <c r="AM240" t="s" s="2">
         <v>609</v>
       </c>
-      <c r="AN228" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO228" t="s" s="2">
+      <c r="AN240" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO240" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO228">
+  <autoFilter ref="A1:AO240">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -29188,7 +30631,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI227">
+  <conditionalFormatting sqref="A2:AI239">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Re-publish with location and Condition examples
</commit_message>
<xml_diff>
--- a/docs/UKCore-Observation.xlsx
+++ b/docs/UKCore-Observation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8907" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8908" uniqueCount="733">
   <si>
     <t>Path</t>
   </si>
@@ -1128,7 +1128,7 @@
     <t>PID-3</t>
   </si>
   <si>
-    <t xml:space="preserve">participation[typeCode=RTGT] </t>
+    <t>participation[typeCode=RTGT]</t>
   </si>
   <si>
     <t>FiveWs.subject</t>
@@ -1719,6 +1719,12 @@
   </si>
   <si>
     <t>In some cases, method can impact results and is thus used for determining whether results can be compared or determining significance of results.</t>
+  </si>
+  <si>
+    <t>Methods for simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-methods</t>
   </si>
   <si>
     <t>OBX-17</t>
@@ -19892,11 +19898,13 @@
         <v>45</v>
       </c>
       <c r="W149" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="X149" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="X149" t="s" s="2">
+        <v>551</v>
+      </c>
       <c r="Y149" t="s" s="2">
-        <v>45</v>
+        <v>552</v>
       </c>
       <c r="Z149" t="s" s="2">
         <v>45</v>
@@ -19935,10 +19943,10 @@
         <v>45</v>
       </c>
       <c r="AL149" t="s" s="2">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="AM149" t="s" s="2">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="AN149" t="s" s="2">
         <v>45</v>
@@ -19949,7 +19957,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -19972,16 +19980,16 @@
         <v>45</v>
       </c>
       <c r="J150" t="s" s="2">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="M150" t="s" s="2">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="N150" s="2"/>
       <c r="O150" t="s" s="2">
@@ -20031,7 +20039,7 @@
         <v>45</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>43</v>
@@ -20049,24 +20057,24 @@
         <v>45</v>
       </c>
       <c r="AK150" t="s" s="2">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="AL150" t="s" s="2">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="AM150" t="s" s="2">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="AN150" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO150" t="s" s="2">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -20181,7 +20189,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -20298,7 +20306,7 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
@@ -20415,7 +20423,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -20532,7 +20540,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -20649,7 +20657,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -20764,7 +20772,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -20881,7 +20889,7 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -21000,7 +21008,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -21119,7 +21127,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -21238,7 +21246,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -21355,7 +21363,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -21470,7 +21478,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -21587,7 +21595,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -21704,7 +21712,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -21727,16 +21735,16 @@
         <v>45</v>
       </c>
       <c r="J165" t="s" s="2">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="K165" t="s" s="2">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="M165" t="s" s="2">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="N165" s="2"/>
       <c r="O165" t="s" s="2">
@@ -21786,7 +21794,7 @@
         <v>45</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>43</v>
@@ -21804,24 +21812,24 @@
         <v>45</v>
       </c>
       <c r="AK165" t="s" s="2">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="AL165" t="s" s="2">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="AM165" t="s" s="2">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="AN165" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO165" t="s" s="2">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21936,7 +21944,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -22053,7 +22061,7 @@
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -22170,7 +22178,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -22287,7 +22295,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -22404,7 +22412,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -22519,7 +22527,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -22636,7 +22644,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -22755,7 +22763,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22874,7 +22882,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22993,7 +23001,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -23110,7 +23118,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -23225,7 +23233,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -23342,7 +23350,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -23459,7 +23467,7 @@
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -23482,19 +23490,19 @@
         <v>45</v>
       </c>
       <c r="J180" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="M180" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="N180" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="O180" t="s" s="2">
         <v>45</v>
@@ -23543,7 +23551,7 @@
         <v>45</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>43</v>
@@ -23555,7 +23563,7 @@
         <v>45</v>
       </c>
       <c r="AI180" t="s" s="2">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="AJ180" t="s" s="2">
         <v>45</v>
@@ -23564,10 +23572,10 @@
         <v>45</v>
       </c>
       <c r="AL180" t="s" s="2">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="AM180" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="AN180" t="s" s="2">
         <v>45</v>
@@ -23578,7 +23586,7 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -23693,7 +23701,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -23810,11 +23818,11 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" t="s" s="2">
@@ -23836,10 +23844,10 @@
         <v>101</v>
       </c>
       <c r="K183" t="s" s="2">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="M183" t="s" s="2">
         <v>104</v>
@@ -23894,7 +23902,7 @@
         <v>45</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>43</v>
@@ -23929,7 +23937,7 @@
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23952,13 +23960,13 @@
         <v>45</v>
       </c>
       <c r="J184" t="s" s="2">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="L184" t="s" s="2">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
@@ -24009,7 +24017,7 @@
         <v>45</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>43</v>
@@ -24018,7 +24026,7 @@
         <v>55</v>
       </c>
       <c r="AH184" t="s" s="2">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="AI184" t="s" s="2">
         <v>67</v>
@@ -24030,10 +24038,10 @@
         <v>45</v>
       </c>
       <c r="AL184" t="s" s="2">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="AM184" t="s" s="2">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="AN184" t="s" s="2">
         <v>45</v>
@@ -24044,7 +24052,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -24067,13 +24075,13 @@
         <v>45</v>
       </c>
       <c r="J185" t="s" s="2">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="M185" s="2"/>
       <c r="N185" s="2"/>
@@ -24124,7 +24132,7 @@
         <v>45</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>43</v>
@@ -24133,7 +24141,7 @@
         <v>55</v>
       </c>
       <c r="AH185" t="s" s="2">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="AI185" t="s" s="2">
         <v>67</v>
@@ -24145,10 +24153,10 @@
         <v>45</v>
       </c>
       <c r="AL185" t="s" s="2">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="AM185" t="s" s="2">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="AN185" t="s" s="2">
         <v>45</v>
@@ -24159,7 +24167,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -24185,16 +24193,16 @@
         <v>143</v>
       </c>
       <c r="K186" t="s" s="2">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="L186" t="s" s="2">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="M186" t="s" s="2">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="N186" t="s" s="2">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="O186" t="s" s="2">
         <v>45</v>
@@ -24222,10 +24230,10 @@
         <v>79</v>
       </c>
       <c r="X186" t="s" s="2">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="Y186" t="s" s="2">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="Z186" t="s" s="2">
         <v>45</v>
@@ -24243,7 +24251,7 @@
         <v>45</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>43</v>
@@ -24261,10 +24269,10 @@
         <v>45</v>
       </c>
       <c r="AK186" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="AL186" t="s" s="2">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="AM186" t="s" s="2">
         <v>492</v>
@@ -24278,7 +24286,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -24304,16 +24312,16 @@
         <v>143</v>
       </c>
       <c r="K187" t="s" s="2">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="L187" t="s" s="2">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="M187" t="s" s="2">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="N187" t="s" s="2">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="O187" t="s" s="2">
         <v>45</v>
@@ -24341,10 +24349,10 @@
         <v>278</v>
       </c>
       <c r="X187" t="s" s="2">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="Y187" t="s" s="2">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="Z187" t="s" s="2">
         <v>45</v>
@@ -24362,7 +24370,7 @@
         <v>45</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>43</v>
@@ -24380,10 +24388,10 @@
         <v>45</v>
       </c>
       <c r="AK187" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="AL187" t="s" s="2">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="AM187" t="s" s="2">
         <v>492</v>
@@ -24397,7 +24405,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -24420,17 +24428,17 @@
         <v>45</v>
       </c>
       <c r="J188" t="s" s="2">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="K188" t="s" s="2">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="L188" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="M188" s="2"/>
       <c r="N188" t="s" s="2">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="O188" t="s" s="2">
         <v>45</v>
@@ -24479,7 +24487,7 @@
         <v>45</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>43</v>
@@ -24503,7 +24511,7 @@
         <v>45</v>
       </c>
       <c r="AM188" t="s" s="2">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="AN188" t="s" s="2">
         <v>45</v>
@@ -24514,7 +24522,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -24540,10 +24548,10 @@
         <v>57</v>
       </c>
       <c r="K189" t="s" s="2">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="L189" t="s" s="2">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="M189" s="2"/>
       <c r="N189" s="2"/>
@@ -24594,7 +24602,7 @@
         <v>45</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>43</v>
@@ -24615,10 +24623,10 @@
         <v>45</v>
       </c>
       <c r="AL189" t="s" s="2">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="AM189" t="s" s="2">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="AN189" t="s" s="2">
         <v>45</v>
@@ -24629,7 +24637,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -24652,16 +24660,16 @@
         <v>56</v>
       </c>
       <c r="J190" t="s" s="2">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="K190" t="s" s="2">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="M190" t="s" s="2">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="N190" s="2"/>
       <c r="O190" t="s" s="2">
@@ -24711,7 +24719,7 @@
         <v>45</v>
       </c>
       <c r="AE190" t="s" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="AF190" t="s" s="2">
         <v>43</v>
@@ -24732,10 +24740,10 @@
         <v>45</v>
       </c>
       <c r="AL190" t="s" s="2">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="AM190" t="s" s="2">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="AN190" t="s" s="2">
         <v>45</v>
@@ -24746,7 +24754,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -24861,7 +24869,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24978,7 +24986,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -25095,7 +25103,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -25212,7 +25220,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -25329,7 +25337,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -25444,7 +25452,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -25561,7 +25569,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -25680,7 +25688,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -25799,7 +25807,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25918,7 +25926,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -26035,7 +26043,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -26150,7 +26158,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -26267,7 +26275,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -26384,7 +26392,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -26407,16 +26415,16 @@
         <v>56</v>
       </c>
       <c r="J205" t="s" s="2">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="K205" t="s" s="2">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="M205" t="s" s="2">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="N205" s="2"/>
       <c r="O205" t="s" s="2">
@@ -26466,7 +26474,7 @@
         <v>45</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>43</v>
@@ -26487,10 +26495,10 @@
         <v>45</v>
       </c>
       <c r="AL205" t="s" s="2">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="AM205" t="s" s="2">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="AN205" t="s" s="2">
         <v>45</v>
@@ -26501,7 +26509,7 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
@@ -26616,7 +26624,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -26733,7 +26741,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -26850,7 +26858,7 @@
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -26967,7 +26975,7 @@
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -27084,7 +27092,7 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
@@ -27199,7 +27207,7 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
@@ -27316,7 +27324,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -27435,7 +27443,7 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -27554,7 +27562,7 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -27673,7 +27681,7 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -27790,7 +27798,7 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -27905,7 +27913,7 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -28022,7 +28030,7 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -28139,7 +28147,7 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" t="s" s="2">
@@ -28162,19 +28170,19 @@
         <v>56</v>
       </c>
       <c r="J220" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="K220" t="s" s="2">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="M220" t="s" s="2">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="N220" t="s" s="2">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="O220" t="s" s="2">
         <v>45</v>
@@ -28223,7 +28231,7 @@
         <v>45</v>
       </c>
       <c r="AE220" t="s" s="2">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="AF220" t="s" s="2">
         <v>43</v>
@@ -28244,10 +28252,10 @@
         <v>45</v>
       </c>
       <c r="AL220" t="s" s="2">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="AM220" t="s" s="2">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="AN220" t="s" s="2">
         <v>45</v>
@@ -28258,7 +28266,7 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
@@ -28373,7 +28381,7 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
@@ -28490,11 +28498,11 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D223" s="2"/>
       <c r="E223" t="s" s="2">
@@ -28516,10 +28524,10 @@
         <v>101</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="M223" t="s" s="2">
         <v>104</v>
@@ -28574,7 +28582,7 @@
         <v>45</v>
       </c>
       <c r="AE223" t="s" s="2">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="AF223" t="s" s="2">
         <v>43</v>
@@ -28609,7 +28617,7 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" t="s" s="2">
@@ -28635,13 +28643,13 @@
         <v>143</v>
       </c>
       <c r="K224" t="s" s="2">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="L224" t="s" s="2">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="M224" t="s" s="2">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="N224" t="s" s="2">
         <v>277</v>
@@ -28693,7 +28701,7 @@
         <v>45</v>
       </c>
       <c r="AE224" t="s" s="2">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="AF224" t="s" s="2">
         <v>55</v>
@@ -28711,7 +28719,7 @@
         <v>45</v>
       </c>
       <c r="AK224" t="s" s="2">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="AL224" t="s" s="2">
         <v>283</v>
@@ -28728,7 +28736,7 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" t="s" s="2">
@@ -28843,7 +28851,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
@@ -28960,7 +28968,7 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
@@ -29077,7 +29085,7 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B228" t="s" s="2">
         <v>299</v>
@@ -29198,7 +29206,7 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B229" s="2"/>
       <c r="C229" t="s" s="2">
@@ -29313,7 +29321,7 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" t="s" s="2">
@@ -29430,7 +29438,7 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" t="s" s="2">
@@ -29549,7 +29557,7 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B232" s="2"/>
       <c r="C232" t="s" s="2">
@@ -29666,7 +29674,7 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B233" s="2"/>
       <c r="C233" t="s" s="2">
@@ -29783,7 +29791,7 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B234" s="2"/>
       <c r="C234" t="s" s="2">
@@ -29900,7 +29908,7 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B235" s="2"/>
       <c r="C235" t="s" s="2">
@@ -30019,7 +30027,7 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B236" s="2"/>
       <c r="C236" t="s" s="2">
@@ -30138,7 +30146,7 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B237" s="2"/>
       <c r="C237" t="s" s="2">
@@ -30164,13 +30172,13 @@
         <v>463</v>
       </c>
       <c r="K237" t="s" s="2">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="L237" t="s" s="2">
         <v>465</v>
       </c>
       <c r="M237" t="s" s="2">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="N237" t="s" s="2">
         <v>467</v>
@@ -30222,7 +30230,7 @@
         <v>45</v>
       </c>
       <c r="AE237" t="s" s="2">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="AF237" t="s" s="2">
         <v>43</v>
@@ -30240,7 +30248,7 @@
         <v>45</v>
       </c>
       <c r="AK237" t="s" s="2">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="AL237" t="s" s="2">
         <v>470</v>
@@ -30257,7 +30265,7 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B238" s="2"/>
       <c r="C238" t="s" s="2">
@@ -30283,13 +30291,13 @@
         <v>143</v>
       </c>
       <c r="K238" t="s" s="2">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="L238" t="s" s="2">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="M238" t="s" s="2">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="N238" t="s" s="2">
         <v>477</v>
@@ -30341,7 +30349,7 @@
         <v>45</v>
       </c>
       <c r="AE238" t="s" s="2">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="AF238" t="s" s="2">
         <v>43</v>
@@ -30376,7 +30384,7 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B239" s="2"/>
       <c r="C239" t="s" s="2">
@@ -30460,7 +30468,7 @@
         <v>45</v>
       </c>
       <c r="AE239" t="s" s="2">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="AF239" t="s" s="2">
         <v>43</v>
@@ -30495,7 +30503,7 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" t="s" s="2">
@@ -30521,16 +30529,16 @@
         <v>45</v>
       </c>
       <c r="K240" t="s" s="2">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="L240" t="s" s="2">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="M240" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="N240" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="O240" t="s" s="2">
         <v>45</v>
@@ -30579,7 +30587,7 @@
         <v>45</v>
       </c>
       <c r="AE240" t="s" s="2">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="AF240" t="s" s="2">
         <v>43</v>
@@ -30600,10 +30608,10 @@
         <v>45</v>
       </c>
       <c r="AL240" t="s" s="2">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="AM240" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="AN240" t="s" s="2">
         <v>45</v>

</xml_diff>